<commit_message>
Chinh sua Ke Hoach
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CSDL\DoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31F6806-B450-4CA1-B0CC-23E6FB6BCAA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D3E6E2-888C-4DA9-9A51-572BEBE5BF37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>b, c</t>
   </si>
   <si>
-    <t xml:space="preserve">                   10/5/2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">*a Viết hàm Mua sản phẩm (theo Tên/Mã và kèm số lượng muốn mua)          *b Viết hàm Xuất hóa đơn (Xuất ra Tên các sản phẩm đã mua, số lượng mỗi sản phẩm, tổng giá tiền mỗi sản phẩm, tổng giá đơn hàng)                                  *c Viết hàm tính Tổng doanh thu bán hàng     </t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>*a Viết hàm Thêm sản phẩm mới vào danh sách (Thêm vào đầu danh sách, thêm vào cuối danh sách, thêm sau một sản phẩm)                                             *b Viết hàm Bổ sung số lượng sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   9/28/2018</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -697,13 +697,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="14">
         <v>43364</v>
@@ -724,17 +724,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="14">
-        <v>43378</v>
+        <v>43371</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -754,10 +754,10 @@
         <v>20</v>
       </c>
       <c r="E7" s="14">
-        <v>43379</v>
+        <v>43372</v>
       </c>
       <c r="F7" s="14">
-        <v>43379</v>
+        <v>43372</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -768,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>21</v>
@@ -777,10 +777,10 @@
         <v>18</v>
       </c>
       <c r="E8" s="14">
-        <v>43385</v>
+        <v>43378</v>
       </c>
       <c r="F8" s="14">
-        <v>43387</v>
+        <v>43380</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -797,13 +797,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="14">
-        <v>43392</v>
+        <v>43385</v>
       </c>
       <c r="F9" s="14">
-        <v>43393</v>
+        <v>43386</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -814,19 +814,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="14">
-        <v>43394</v>
+        <v>43387</v>
       </c>
       <c r="F10" s="14">
-        <v>43394</v>
+        <v>43387</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -840,16 +840,16 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="14">
-        <v>43399</v>
+        <v>43392</v>
       </c>
       <c r="F11" s="14">
-        <v>43401</v>
+        <v>43394</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -863,16 +863,16 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="14">
-        <v>43406</v>
+        <v>43399</v>
       </c>
       <c r="F12" s="14">
-        <v>43407</v>
+        <v>43400</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -886,16 +886,16 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="14">
+        <v>43401</v>
+      </c>
+      <c r="F13" s="14">
         <v>43408</v>
-      </c>
-      <c r="F13" s="14">
-        <v>43415</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>

</xml_diff>

<commit_message>
Khang chinh sua lai thoi gian ke hoach va lam menu chuc nang!
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CSDL\DoAn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CTDL\DoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D3E6E2-888C-4DA9-9A51-572BEBE5BF37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06E9A10-5D2D-40A5-9960-7F29035ED11E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>*a Viết hàm Thêm sản phẩm mới vào danh sách (Thêm vào đầu danh sách, thêm vào cuối danh sách, thêm sau một sản phẩm)                                             *b Viết hàm Bổ sung số lượng sản phẩm</t>
   </si>
   <si>
-    <t xml:space="preserve">                   9/28/2018</t>
+    <t xml:space="preserve">                   10/5/2018</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -652,16 +652,16 @@
         <v>4</v>
       </c>
       <c r="E3" s="14">
-        <v>43351</v>
+        <v>43357</v>
       </c>
       <c r="F3" s="14">
-        <v>43353</v>
+        <v>43359</v>
       </c>
       <c r="G3" s="14">
-        <v>43352</v>
+        <v>43357</v>
       </c>
       <c r="H3" s="14">
-        <v>43353</v>
+        <v>43358</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -679,16 +679,16 @@
         <v>4</v>
       </c>
       <c r="E4" s="14">
-        <v>43354</v>
+        <v>43359</v>
       </c>
       <c r="F4" s="14">
-        <v>43355</v>
+        <v>43359</v>
       </c>
       <c r="G4" s="14">
-        <v>43354</v>
+        <v>43359</v>
       </c>
       <c r="H4" s="14">
-        <v>43354</v>
+        <v>43359</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -706,16 +706,16 @@
         <v>27</v>
       </c>
       <c r="E5" s="14">
-        <v>43364</v>
+        <v>43371</v>
       </c>
       <c r="F5" s="14">
-        <v>43366</v>
+        <v>43373</v>
       </c>
       <c r="G5" s="14">
-        <v>43365</v>
+        <v>43372</v>
       </c>
       <c r="H5" s="14">
-        <v>43366</v>
+        <v>43373</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -731,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="14">
-        <v>43371</v>
+        <v>43378</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>30</v>
@@ -754,10 +754,10 @@
         <v>20</v>
       </c>
       <c r="E7" s="14">
-        <v>43372</v>
+        <v>43379</v>
       </c>
       <c r="F7" s="14">
-        <v>43372</v>
+        <v>43380</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -777,10 +777,10 @@
         <v>18</v>
       </c>
       <c r="E8" s="14">
-        <v>43378</v>
+        <v>43386</v>
       </c>
       <c r="F8" s="14">
-        <v>43380</v>
+        <v>43387</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -800,10 +800,10 @@
         <v>23</v>
       </c>
       <c r="E9" s="14">
-        <v>43385</v>
+        <v>43387</v>
       </c>
       <c r="F9" s="14">
-        <v>43386</v>
+        <v>43388</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -823,10 +823,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="14">
-        <v>43387</v>
+        <v>43393</v>
       </c>
       <c r="F10" s="14">
-        <v>43387</v>
+        <v>43394</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -846,10 +846,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="14">
-        <v>43392</v>
+        <v>43399</v>
       </c>
       <c r="F11" s="14">
-        <v>43394</v>
+        <v>43400</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -869,10 +869,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="14">
-        <v>43399</v>
+        <v>43401</v>
       </c>
       <c r="F12" s="14">
-        <v>43400</v>
+        <v>43402</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>

</xml_diff>

<commit_message>
Cap nhat tien do
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CTDL\DoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCA6DDD-800D-486D-AC47-CDE0A4335416}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC16E5-ED10-43D2-B278-61AC53914011}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -741,8 +741,12 @@
       <c r="F6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="14">
+        <v>43383</v>
+      </c>
+      <c r="H6" s="14">
+        <v>43383</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -764,8 +768,12 @@
       <c r="F7" s="14">
         <v>43380</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="14">
+        <v>43384</v>
+      </c>
+      <c r="H7" s="14">
+        <v>43384</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
@@ -787,8 +795,12 @@
       <c r="F8" s="14">
         <v>43387</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="14">
+        <v>43386</v>
+      </c>
+      <c r="H8" s="14">
+        <v>43386</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Bo sung ke hoach (them mot so chuc nang)
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CTDL\DoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC16E5-ED10-43D2-B278-61AC53914011}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A4B263-94C7-4A7A-806F-8DCC9588DB72}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -95,58 +95,68 @@
     <t>* Kiểm tra, sửa lỗi, tinh chỉnh, bổ sung chương trình (nếu có)</t>
   </si>
   <si>
-    <t>* Thiết kế giao diện đơn giản cho chương trình</t>
-  </si>
-  <si>
-    <t>* Kiểm tra, sửa lỗi, bổ sung và hoàn thiện chương trình</t>
-  </si>
-  <si>
-    <t>* Viết báo cáo đồ án với Word và Powerpoint</t>
-  </si>
-  <si>
-    <t>*a Viết hàm Xóa sản phẩm khỏi danh sách (Yêu cầu nhập Mã sản phẩm)            *b Viết hàm Kiểm tra trạng thái sản phẩm (theo Tên/Mã sản phẩm)                *c Viết hàm Tìm kiếm sản phẩm (theo Tên, theo Mã, theo Khoảng giá)</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>a, b</t>
   </si>
   <si>
-    <t xml:space="preserve">             c</t>
-  </si>
-  <si>
-    <t>b, c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*a Viết hàm Mua sản phẩm (theo Tên/Mã và kèm số lượng muốn mua)          *b Viết hàm Xuất hóa đơn (Xuất ra Tên các sản phẩm đã mua, số lượng mỗi sản phẩm, tổng giá tiền mỗi sản phẩm, tổng giá đơn hàng)                                  *c Viết hàm tính Tổng doanh thu bán hàng     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">             x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Lên ý tưởng và tìm hiểu về tạo giao diện dựa vào các hàm đồ họa        </t>
-  </si>
-  <si>
-    <t>a, b, d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c, e, f                      </t>
-  </si>
-  <si>
-    <t>*a Khai báo struct cho sản phẩm                                                                               *b Viết hàm tạo danh sách sản phẩm                                                                       *c Viết hàm nhập các sản phẩm vào danh sách                                                     *d Viết hàm xuất danh sách các sản phẩm (xuất ra đầy đủ Mã sản phẩm, Tên sản phẩm, Giá bán, Số lượng, Ngày sản xuất, Hạn sử dụng, Nhà cung cấp)                                                                                                                         *e Tạo Menu gồm các chức năng: Thêm sản phẩm mới, Bổ sung Số lượng sản phẩm, Xóa sản phẩm khỏi danh sách, Tìm kiếm sản phẩm, Kiểm tra trạng thái sản phẩm, Mua sản phẩm, Xuất hóa đơn, Tổng doanh thu bán hàng                                                                                                                          *f Viết hàm giải phóng bộ nhớ</t>
-  </si>
-  <si>
-    <t>*a Viết hàm Thêm sản phẩm mới vào danh sách (Thêm vào đầu danh sách, thêm vào cuối danh sách, thêm sau một sản phẩm)                                             *b Viết hàm Bổ sung số lượng sản phẩm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                   10/5/2018</t>
-  </si>
-  <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>*a Viết chức năng Thêm sản phẩm mới vào danh sách (Thêm vào đầu danh sách, thêm vào cuối danh sách, thêm sau một sản phẩm)
+*b Viết chức năng Bổ sung số lượng sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*a Viết chức năng Mua sản phẩm (theo Tên/Mã và kèm số lượng muốn mua)
+*b Viết chức năng Xuất hóa đơn (Xuất ra Tên các sản phẩm đã mua, số lượng mỗi sản phẩm, tổng giá tiền mỗi sản phẩm, tổng giá đơn hàng)
+*c Viết chức năng tính Tổng doanh thu bán hàng     </t>
+  </si>
+  <si>
+    <t>*a Viết chức năng Khuyến mãi
+*b Viết chức năng Trả hàng
+*c  Viết chức năng Thối tiền
+*d  Viết chức năng Sắp xếp sản phẩm theo giá bán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*a Viết chức năng Kiểm tra các sản phẩm đã được bán kèm theo sản phẩm bán chạy nhất
+*b Viết chức năng Kiểm tra các mặt hàng đã hết hạn sử dụng
+*c  Viết chức năng Lợi nhuận
+</t>
+  </si>
+  <si>
+    <t>*a Viết chức năng Xóa sản phẩm khỏi danh sách (Yêu cầu nhập Mã sản phẩm)
+*b Viết chức năng Tìm kiếm sản phẩm (theo Tên, theo Mã, theo Khoảng giá)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
+  <si>
+    <t>*a Khai báo struct cho sản phẩm                                                                              *b Viết hàm tạo danh sách sản phẩm
+*c Viết hàm nhập các sản phẩm vào danh sách (từ File)
+*d Viết hàm xuất danh sách các sản phẩm (xuất ra đầy đủ Mã sản phẩm, Tên sản phẩm, Giá bán, Số lượng, Ngày sản xuất, Hạn sử dụng, Nhà cung cấp)
+*e Tạo Menu gồm các chức năng: Thêm sản phẩm mới, Bổ sung Số lượng sản phẩm, Xóa sản phẩm khỏi danh sách, Tìm kiếm sản phẩm, Mua sản phẩm, Xuất hóa đơn, Khuyến mãi, Trả hàng, Thối tiền, Sắp xếp sản phẩm theo giá bán, Kiểm tra các sản phẩm đã được bán kèm theo sản phẩm bán chạy nhất, Kiểm tra các mặt hàng đã hết hạn sử dụng, Tổng doanh thu bán hàng, Lợi nhuận
+*f Viết hàm giải phóng bộ nhớ</t>
+  </si>
+  <si>
+    <t>a, b, c, d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e, f                   </t>
+  </si>
+  <si>
+    <t>a, c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c, d                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Lên ý tưởng và tìm hiểu về tạo giao diện dựa vào các hàm đồ họa
+* Thiết kế giao diện đơn giản cho chương trình       </t>
+  </si>
+  <si>
+    <t>* Kiểm tra, sửa lỗi, bổ sung và hoàn thiện chương trình
+* Viết báo cáo đồ án với Word và Powerpoint</t>
   </si>
 </sst>
 </file>
@@ -256,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,8 +306,26 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -641,83 +669,83 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="18">
         <v>43357</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="18">
         <v>43359</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="18">
         <v>43357</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="18">
         <v>43358</v>
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="18">
         <v>43359</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="18">
         <v>43359</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="18">
         <v>43359</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="18">
         <v>43359</v>
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="158.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="193.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="14">
+        <v>23</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="18">
         <v>43371</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="18">
         <v>43373</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="18">
         <v>43372</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="18">
         <v>43373</v>
       </c>
       <c r="I5" s="3"/>
@@ -727,52 +755,52 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="14">
-        <v>43378</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="14">
-        <v>43383</v>
-      </c>
-      <c r="H6" s="14">
-        <v>43383</v>
+        <v>17</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18">
+        <v>43385</v>
+      </c>
+      <c r="F6" s="18">
+        <v>43386</v>
+      </c>
+      <c r="G6" s="18">
+        <v>43386</v>
+      </c>
+      <c r="H6" s="18">
+        <v>43387</v>
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="14">
-        <v>43379</v>
-      </c>
-      <c r="F7" s="14">
-        <v>43380</v>
-      </c>
-      <c r="G7" s="14">
-        <v>43384</v>
-      </c>
-      <c r="H7" s="14">
-        <v>43384</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18">
+        <v>43387</v>
+      </c>
+      <c r="F7" s="18">
+        <v>43389</v>
+      </c>
+      <c r="G7" s="18">
+        <v>43387</v>
+      </c>
+      <c r="H7" s="18">
+        <v>43389</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -781,218 +809,214 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="14">
-        <v>43386</v>
-      </c>
-      <c r="F8" s="14">
-        <v>43387</v>
-      </c>
-      <c r="G8" s="14">
-        <v>43386</v>
-      </c>
-      <c r="H8" s="14">
-        <v>43386</v>
-      </c>
+      <c r="C8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="18">
+        <v>43392</v>
+      </c>
+      <c r="F8" s="18">
+        <v>43392</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="14">
-        <v>43387</v>
-      </c>
-      <c r="F9" s="14">
-        <v>43388</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="21">
+        <v>43394</v>
+      </c>
+      <c r="F9" s="21">
+        <v>43397</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="61.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="14">
-        <v>43393</v>
-      </c>
-      <c r="F10" s="14">
-        <v>43394</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="21">
+        <v>43399</v>
+      </c>
+      <c r="F10" s="21">
+        <v>43399</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="14">
-        <v>43399</v>
-      </c>
-      <c r="F11" s="14">
+      <c r="D11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="21">
         <v>43400</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="F11" s="21">
+        <v>43401</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="14">
-        <v>43401</v>
-      </c>
-      <c r="F12" s="14">
-        <v>43402</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="D12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="21">
+        <v>43406</v>
+      </c>
+      <c r="F12" s="21">
+        <v>43409</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="B13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="14">
-        <v>43401</v>
-      </c>
-      <c r="F13" s="14">
-        <v>43408</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="D13" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="21">
+        <v>43413</v>
+      </c>
+      <c r="F13" s="21">
+        <v>43415</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Cap nhat tien do ke hoach
</commit_message>
<xml_diff>
--- a/KeHoach.xlsx
+++ b/KeHoach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\CTDL&amp;GT\DoAn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang\Desktop\New folder\DoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFEACEE-E1F5-4111-89AF-4CAB0D2DDF51}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F27D40A-A9EE-4613-B765-35EB15BC0D65}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -961,7 +961,9 @@
       <c r="G13" s="18">
         <v>43413</v>
       </c>
-      <c r="H13" s="18"/>
+      <c r="H13" s="18">
+        <v>43433</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">

</xml_diff>